<commit_message>
change dm fields naming convention
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/registration_datahub/tests/test_file/rdi_import_1_hh_10_people_missing_required_delivery_fields.xlsx
+++ b/backend/hct_mis_api/apps/registration_datahub/tests/test_file/rdi_import_1_hh_10_people_missing_required_delivery_fields.xlsx
@@ -825,13 +825,13 @@
     <t>pp_country_i_c</t>
   </si>
   <si>
-    <t>pp_card_number_atm_card_i_c</t>
-  </si>
-  <si>
-    <t>pp_card_expiry_date_atm_card_i_c</t>
-  </si>
-  <si>
-    <t>pp_name_of_cardholder_atm_card_i_c</t>
+    <t>pp_card_number__atm_card_i_c</t>
+  </si>
+  <si>
+    <t>pp_card_expiry_date__atm_card_i_c</t>
+  </si>
+  <si>
+    <t>pp_name_of_cardholder__atm_card_i_c</t>
   </si>
   <si>
     <t>Samuel Russell</t>
@@ -4536,7 +4536,10 @@
     <col min="1" max="65" width="8.85156" style="7" customWidth="1"/>
     <col min="66" max="66" width="10.1719" style="7" customWidth="1"/>
     <col min="67" max="67" width="22.5" style="7" customWidth="1"/>
-    <col min="68" max="76" width="8.85156" style="7" customWidth="1"/>
+    <col min="68" max="73" width="8.85156" style="7" customWidth="1"/>
+    <col min="74" max="74" width="30.1953" style="7" customWidth="1"/>
+    <col min="75" max="75" width="34.9688" style="7" customWidth="1"/>
+    <col min="76" max="76" width="30.5" style="7" customWidth="1"/>
     <col min="77" max="16384" width="8.85156" style="7" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>